<commit_message>
Update module bill and cotizaciones
</commit_message>
<xml_diff>
--- a/assets/formatos/facturadefault.xlsx
+++ b/assets/formatos/facturadefault.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\lotus\assets\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3235F6B2-4E0B-450C-9911-0686B2F0A5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2438DB9-A8DC-48B7-9A17-9A4913620158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23028" yWindow="0" windowWidth="21624" windowHeight="11304" xr2:uid="{9937E0F9-D6B8-4033-8F9C-169D8685DA2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9937E0F9-D6B8-4033-8F9C-169D8685DA2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Factura" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>Datos del emisor</t>
   </si>
@@ -105,10 +105,6 @@
   </si>
   <si>
     <t xml:space="preserve">N° </t>
-  </si>
-  <si>
-    <t>Sujeto a variación de precio y stock.
-Cotización válida hasta 30.05.2023</t>
   </si>
   <si>
     <t>Subtotal PU</t>
@@ -305,31 +301,22 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -341,13 +328,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -874,8 +870,8 @@
   </sheetPr>
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34:R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,164 +893,164 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
     </row>
     <row r="5" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
     </row>
     <row r="6" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="13">
+      <c r="C6" s="20"/>
+      <c r="D6" s="19">
         <v>348734834734</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
     </row>
     <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
     </row>
     <row r="8" spans="1:19" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
     </row>
     <row r="9" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.8">
       <c r="D9" s="5" t="s">
@@ -1063,21 +1059,21 @@
       <c r="E9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
+      <c r="F9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
     </row>
     <row r="10" spans="1:19" ht="28.5" x14ac:dyDescent="0.8">
       <c r="D10" s="5" t="s">
@@ -1086,21 +1082,21 @@
       <c r="E10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="18">
         <v>0</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
     </row>
     <row r="11" spans="1:19" ht="28.5" x14ac:dyDescent="0.8">
       <c r="D11" s="5" t="s">
@@ -1109,21 +1105,21 @@
       <c r="E11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
+      <c r="F11" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
     </row>
     <row r="12" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.8">
       <c r="D12" s="5" t="s">
@@ -1132,61 +1128,61 @@
       <c r="E12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="18">
         <v>3132093326</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
     </row>
     <row r="13" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
     </row>
     <row r="14" spans="1:19" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="1:19" ht="28.5" x14ac:dyDescent="0.8">
@@ -1196,24 +1192,24 @@
       <c r="E15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
       <c r="L15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N15" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
+      <c r="N15" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
       <c r="S15" s="2"/>
     </row>
     <row r="16" spans="1:19" ht="28.5" x14ac:dyDescent="0.8">
@@ -1223,22 +1219,22 @@
       <c r="E16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
       <c r="L16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
       <c r="S16" s="2"/>
     </row>
     <row r="17" spans="1:19" ht="28.5" x14ac:dyDescent="0.8">
@@ -1248,22 +1244,22 @@
       <c r="E17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
       <c r="L17" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
       <c r="S17" s="2"/>
     </row>
     <row r="18" spans="1:19" ht="28.5" x14ac:dyDescent="0.8">
@@ -1273,22 +1269,22 @@
       <c r="E18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
       <c r="L18" s="5" t="s">
         <v>12</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
       <c r="S18" s="2"/>
     </row>
     <row r="19" spans="1:19" ht="28.5" x14ac:dyDescent="0.8">
@@ -1298,95 +1294,95 @@
       <c r="E19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
       <c r="L19" s="5" t="s">
         <v>13</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
       <c r="S19" s="2"/>
     </row>
     <row r="20" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
     </row>
     <row r="21" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22" t="s">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22" t="s">
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="22"/>
-      <c r="J21" s="21" t="s">
+      <c r="I21" s="10"/>
+      <c r="J21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21" t="s">
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22" t="s">
+      <c r="N21" s="10"/>
+      <c r="O21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="21" t="s">
+      <c r="P21" s="10"/>
+      <c r="Q21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="R21" s="21"/>
+      <c r="R21" s="8"/>
     </row>
     <row r="22" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
     </row>
     <row r="23" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
@@ -1803,212 +1799,397 @@
       <c r="N44" s="7"/>
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="8"/>
+      <c r="Q44" s="22"/>
+      <c r="R44" s="22"/>
     </row>
     <row r="45" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="16"/>
-      <c r="J45" s="16"/>
-      <c r="K45" s="16"/>
-      <c r="L45" s="16"/>
-      <c r="M45" s="16"/>
-      <c r="N45" s="16"/>
-      <c r="O45" s="16"/>
-      <c r="P45" s="16"/>
-      <c r="Q45" s="16"/>
-      <c r="R45" s="16"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="9"/>
-      <c r="R46" s="9"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="18" t="s">
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="L47" s="20"/>
-      <c r="M47" s="20"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
       <c r="N47" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O47" s="17">
+      <c r="O47" s="14">
         <v>1686460</v>
       </c>
-      <c r="P47" s="17"/>
-      <c r="Q47" s="17"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="L48" s="20"/>
-      <c r="M48" s="20"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
       <c r="N48" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O48" s="17">
+      <c r="O48" s="14">
         <v>0</v>
       </c>
-      <c r="P48" s="17"/>
-      <c r="Q48" s="17"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
     </row>
     <row r="49" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
-      <c r="I49" s="19"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="L49" s="20"/>
-      <c r="M49" s="20"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
       <c r="N49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O49" s="17">
+      <c r="O49" s="14">
         <v>1686460</v>
       </c>
-      <c r="P49" s="17"/>
-      <c r="Q49" s="17"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="14"/>
     </row>
     <row r="50" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
       <c r="N50" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O50" s="17">
+      <c r="O50" s="14">
         <v>320427</v>
       </c>
-      <c r="P50" s="17"/>
-      <c r="Q50" s="17"/>
+      <c r="P50" s="14"/>
+      <c r="Q50" s="14"/>
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
       <c r="N51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O51" s="17">
+      <c r="O51" s="14">
         <v>2006887</v>
       </c>
-      <c r="P51" s="17"/>
-      <c r="Q51" s="17"/>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="14"/>
     </row>
     <row r="52" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-      <c r="K52" s="15"/>
-      <c r="L52" s="15"/>
-      <c r="M52" s="15"/>
-      <c r="N52" s="15"/>
-      <c r="O52" s="15"/>
-      <c r="P52" s="15"/>
-      <c r="Q52" s="15"/>
-      <c r="R52" s="15"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="11"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11"/>
+      <c r="Q52" s="11"/>
+      <c r="R52" s="11"/>
     </row>
     <row r="53" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
-      <c r="P53" s="15"/>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="15"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="11"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="Q53" s="11"/>
+      <c r="R53" s="11"/>
     </row>
     <row r="56" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="211">
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="O43:P43"/>
+    <mergeCell ref="Q43:R43"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O40:P40"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="O39:P39"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="J36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="A20:R20"/>
+    <mergeCell ref="C8:R8"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M21:N22"/>
+    <mergeCell ref="O21:P22"/>
+    <mergeCell ref="Q21:R22"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="K1:R5"/>
+    <mergeCell ref="N19:R19"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="B1:J5"/>
+    <mergeCell ref="D6:R6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A7:R7"/>
+    <mergeCell ref="A13:R13"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="N16:R16"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="C14:R14"/>
+    <mergeCell ref="N15:R15"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="N18:R18"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="M52:N53"/>
+    <mergeCell ref="O52:P53"/>
+    <mergeCell ref="Q52:R53"/>
+    <mergeCell ref="B45:R46"/>
+    <mergeCell ref="O50:Q50"/>
+    <mergeCell ref="O51:Q51"/>
+    <mergeCell ref="E47:I49"/>
+    <mergeCell ref="B47:D51"/>
+    <mergeCell ref="E50:J51"/>
+    <mergeCell ref="J47:J49"/>
+    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="B52:D53"/>
+    <mergeCell ref="E52:G53"/>
+    <mergeCell ref="H52:I53"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="K52:L53"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="O47:Q47"/>
+    <mergeCell ref="O48:Q48"/>
+    <mergeCell ref="O49:Q49"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:R28"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="H23:I23"/>
@@ -2033,193 +2214,6 @@
     <mergeCell ref="Q29:R29"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="E28:G28"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="M52:N53"/>
-    <mergeCell ref="O52:P53"/>
-    <mergeCell ref="Q52:R53"/>
-    <mergeCell ref="B45:R46"/>
-    <mergeCell ref="O50:Q50"/>
-    <mergeCell ref="O51:Q51"/>
-    <mergeCell ref="E47:I49"/>
-    <mergeCell ref="B47:D51"/>
-    <mergeCell ref="E50:J51"/>
-    <mergeCell ref="J47:J49"/>
-    <mergeCell ref="K47:M47"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="K49:M49"/>
-    <mergeCell ref="B52:D53"/>
-    <mergeCell ref="E52:G53"/>
-    <mergeCell ref="H52:I53"/>
-    <mergeCell ref="J52:J53"/>
-    <mergeCell ref="K52:L53"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="O47:Q47"/>
-    <mergeCell ref="O48:Q48"/>
-    <mergeCell ref="O49:Q49"/>
-    <mergeCell ref="K1:R5"/>
-    <mergeCell ref="N19:R19"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="B1:J5"/>
-    <mergeCell ref="D6:R6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A7:R7"/>
-    <mergeCell ref="A13:R13"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="N16:R16"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="C14:R14"/>
-    <mergeCell ref="N15:R15"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="N18:R18"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="A20:R20"/>
-    <mergeCell ref="C8:R8"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M21:N22"/>
-    <mergeCell ref="O21:P22"/>
-    <mergeCell ref="Q21:R22"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:L35"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="Q35:R35"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="J36:L36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="O39:P39"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="O40:P40"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="O43:P43"/>
-    <mergeCell ref="Q43:R43"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="M42:N42"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>